<commit_message>
System tests Avanzamento e introduzione nuovi SyT
</commit_message>
<xml_diff>
--- a/src/tests/system_testing_GUIDO/Mapping system test GUIDO.xlsx
+++ b/src/tests/system_testing_GUIDO/Mapping system test GUIDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescomariatorino/Desktop/Università - 0522501879/GitProject/GUIDO/src/tests/system_testing_GUIDO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F8433-5720-884B-A5A7-90A423FF753C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B7E2BC-B84F-E74E-8261-963FA24D7DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
   <si>
     <t>Categoria</t>
   </si>
@@ -463,6 +463,15 @@
   <si>
     <t>Repository: https://github.com/netty/netty
 Data fine: 12/06/2025</t>
+  </si>
+  <si>
+    <t>SYSTE-17</t>
+  </si>
+  <si>
+    <t>SYSTE-18</t>
+  </si>
+  <si>
+    <t>Sezione Graph</t>
   </si>
 </sst>
 </file>
@@ -884,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1293,7 @@
     </row>
     <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>10</v>
@@ -1305,7 +1314,7 @@
     </row>
     <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
@@ -1326,10 +1335,10 @@
     </row>
     <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>25</v>
@@ -1347,10 +1356,10 @@
     </row>
     <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -1368,10 +1377,10 @@
     </row>
     <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>25</v>
@@ -1384,6 +1393,27 @@
         <v>36</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avanzamento system test e pubblicazione documentazione system tests
</commit_message>
<xml_diff>
--- a/src/tests/system_testing_GUIDO/Mapping system test GUIDO.xlsx
+++ b/src/tests/system_testing_GUIDO/Mapping system test GUIDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescomariatorino/Desktop/Università - 0522501879/GitProject/GUIDO/src/tests/system_testing_GUIDO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B7E2BC-B84F-E74E-8261-963FA24D7DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4335BC03-3536-D047-B0C8-D0509495945A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Categoria</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Data richiesta</t>
   </si>
   <si>
-    <t>Visualizzazione richieste</t>
-  </si>
-  <si>
     <t>Visualizzazione pending</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>Insufficienti</t>
   </si>
   <si>
-    <t>Visualizza le proprie richieste</t>
-  </si>
-  <si>
     <t>Richiesta in attesa</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Errore specifico: dati non sufficienti</t>
   </si>
   <si>
-    <t>Sezione accessibile</t>
-  </si>
-  <si>
     <t>Appare tra le pending</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
   </si>
   <si>
     <t>Empty</t>
-  </si>
-  <si>
-    <t>Convalide usabilità</t>
   </si>
   <si>
     <t>Repo_valida</t>
@@ -371,10 +359,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t xml:space="preserve">Repository: 
-Data fine: </t>
-  </si>
-  <si>
     <t>Repository: http://google.com/user/repo
 Data fine: 29/06/2025</t>
   </si>
@@ -468,17 +452,18 @@
     <t>SYSTE-17</t>
   </si>
   <si>
-    <t>SYSTE-18</t>
-  </si>
-  <si>
     <t>Sezione Graph</t>
+  </si>
+  <si>
+    <t>Repository: https://github.com/angular/angular
+Data fine: 01/01/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,31 +498,18 @@
       <name val="Calibri (Corpo)"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -568,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,12 +552,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -893,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A21" sqref="A21:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -921,348 +887,348 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>63</v>
+        <v>31</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,151 +1240,129 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{45FB4B78-FFCB-A54C-9173-FF7F2B6B0C98}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{5C2CCDE2-B261-6E41-8D71-70E83B5C14BE}"/>

</xml_diff>